<commit_message>
Se crea el componente CreateManySuppliers para creacion masiva de proveedores
</commit_message>
<xml_diff>
--- a/public/DownloadExcels/Clientes.xlsx
+++ b/public/DownloadExcels/Clientes.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos Mario\Desktop\Ecopcion Desarrollo\ecopFront-Desarrollo\public\DownloadExcels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos Reyes\OneDrive - Top Drive Group\Escritorio\CARLOS\Desarrollo\ecopFront-Desarrollo\public\DownloadExcels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2560EDB5-DFDF-4553-A26F-93F16ECD0574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{073ECB1C-DB9D-4B86-908D-8AC0A0811967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="28800" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIENTES" sheetId="1" r:id="rId1"/>
     <sheet name="INSTRUCCIONES" sheetId="3" r:id="rId2"/>
-    <sheet name="Lista desplegable" sheetId="2" r:id="rId3"/>
+    <sheet name="Lista desplegable" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -4167,7 +4167,7 @@
   <dimension ref="A1:L998"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Formateo de archivos Excel descargables para creacion masiva
</commit_message>
<xml_diff>
--- a/public/DownloadExcels/Clientes.xlsx
+++ b/public/DownloadExcels/Clientes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos Reyes\OneDrive - Top Drive Group\Escritorio\CARLOS\Desarrollo\ecopFront-Desarrollo\public\DownloadExcels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0C2689-B244-4712-A88A-7D918CEAD3A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF2AC9A-6F6D-4BDD-A096-7B36E4E79B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIENTES" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="1097">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1182" uniqueCount="1090">
   <si>
     <t>Instrucciones para diligenciar el formulario</t>
   </si>
@@ -3518,27 +3518,6 @@
     <t>No es obligatorio, si tu cliente tiene dígito de verificación, diligenciar este espacio
 Ej: 1
 Ej: 2</t>
-  </si>
-  <si>
-    <t>FELIPE</t>
-  </si>
-  <si>
-    <t>HERNANDEZ</t>
-  </si>
-  <si>
-    <t>EL COMERCIO SA</t>
-  </si>
-  <si>
-    <t>felipe@gmail.com</t>
-  </si>
-  <si>
-    <t>elcomercio@gmail.com</t>
-  </si>
-  <si>
-    <t>Cra 10</t>
-  </si>
-  <si>
-    <t>Cra 20</t>
   </si>
 </sst>
 </file>
@@ -4188,22 +4167,22 @@
   <dimension ref="A1:L998"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" customWidth="1"/>
-    <col min="2" max="2" width="32.109375" customWidth="1"/>
-    <col min="3" max="3" width="32.5546875" customWidth="1"/>
-    <col min="4" max="4" width="32.6640625" customWidth="1"/>
-    <col min="5" max="5" width="22.109375" customWidth="1"/>
-    <col min="6" max="6" width="31.44140625" customWidth="1"/>
-    <col min="7" max="7" width="31.6640625" customWidth="1"/>
-    <col min="8" max="8" width="35.109375" customWidth="1"/>
-    <col min="9" max="9" width="31.44140625" customWidth="1"/>
-    <col min="10" max="12" width="31.5546875" customWidth="1"/>
-    <col min="13" max="26" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" customWidth="1"/>
+    <col min="3" max="3" width="32.5703125" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="31.42578125" customWidth="1"/>
+    <col min="7" max="7" width="31.7109375" customWidth="1"/>
+    <col min="8" max="8" width="35.140625" customWidth="1"/>
+    <col min="9" max="9" width="31.42578125" customWidth="1"/>
+    <col min="10" max="12" width="31.5703125" customWidth="1"/>
+    <col min="13" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="37.5" customHeight="1">
@@ -4300,35 +4279,17 @@
       <c r="A4" s="6">
         <v>1</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>1090</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>1091</v>
-      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
       <c r="D4" s="11"/>
-      <c r="E4" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="14">
-        <v>121212121</v>
-      </c>
+      <c r="E4" s="11"/>
+      <c r="F4" s="14"/>
       <c r="G4" s="11"/>
-      <c r="H4" s="23" t="s">
-        <v>1093</v>
-      </c>
-      <c r="I4" s="11">
-        <v>3100200323</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>1057</v>
-      </c>
-      <c r="K4" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="L4" s="13" t="s">
-        <v>1095</v>
-      </c>
+      <c r="H4" s="23"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="13"/>
     </row>
     <row r="5" spans="1:12" ht="14.25" customHeight="1">
       <c r="A5" s="6">
@@ -4336,33 +4297,15 @@
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
-      <c r="D5" s="11" t="s">
-        <v>1092</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>1072</v>
-      </c>
-      <c r="F5" s="14">
-        <v>890890890</v>
-      </c>
-      <c r="G5" s="11">
-        <v>5</v>
-      </c>
-      <c r="H5" s="23" t="s">
-        <v>1094</v>
-      </c>
-      <c r="I5" s="11">
-        <v>6012030</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="12" t="s">
-        <v>545</v>
-      </c>
-      <c r="L5" s="13" t="s">
-        <v>1096</v>
-      </c>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="13"/>
     </row>
     <row r="6" spans="1:12" ht="14.25" customHeight="1">
       <c r="A6" s="6">
@@ -18666,13 +18609,9 @@
   <mergeCells count="1">
     <mergeCell ref="A1:L1"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="H4" r:id="rId1" xr:uid="{CEF17AA2-8648-4835-90A7-C44EC9A50701}"/>
-    <hyperlink ref="H5" r:id="rId2" xr:uid="{1A944A30-EC6A-44B9-A72A-48959FABBCDC}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
@@ -18708,7 +18647,7 @@
       <selection activeCell="A2" sqref="A2:K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" customHeight="1">
       <c r="A1" s="25" t="s">
@@ -18757,14 +18696,14 @@
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
     <col min="4" max="4" width="29" customWidth="1"/>
-    <col min="5" max="8" width="10.6640625" customWidth="1"/>
-    <col min="10" max="25" width="10.6640625" customWidth="1"/>
+    <col min="5" max="8" width="10.7109375" customWidth="1"/>
+    <col min="10" max="25" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Ajustes en formularios de creacion masiva
</commit_message>
<xml_diff>
--- a/public/DownloadExcels/Clientes.xlsx
+++ b/public/DownloadExcels/Clientes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos Reyes\OneDrive - Top Drive Group\Escritorio\CARLOS\Desarrollo\ecopFront-Desarrollo\public\DownloadExcels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos Reyes\OneDrive - Top Drive Group\Escritorio\Carlos\Desarrollo\ecopFront-Desarrollo\public\DownloadExcels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF2AC9A-6F6D-4BDD-A096-7B36E4E79B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD38E50-8AAA-40D3-9C8E-297EE1888718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CLIENTES" sheetId="1" r:id="rId1"/>
@@ -4167,7 +4167,7 @@
   <dimension ref="A1:L998"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Ingresos pendientes de aprobar
</commit_message>
<xml_diff>
--- a/public/DownloadExcels/Clientes.xlsx
+++ b/public/DownloadExcels/Clientes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos Reyes\OneDrive - Top Drive Group\Escritorio\Carlos\Desarrollo\ecopFront-Desarrollo\public\DownloadExcels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://topdrive-my.sharepoint.com/personal/carlos_reyes_topdrivegroup_com/Documents/Escritorio/Carlos/Desarrollo/ecopFront-Desarrollo/public/DownloadExcels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD38E50-8AAA-40D3-9C8E-297EE1888718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{8DD38E50-8AAA-40D3-9C8E-297EE1888718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2DD69F7-DF62-41EA-9AD3-842A0D4DC700}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4167,7 +4167,7 @@
   <dimension ref="A1:L998"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4328,7 +4328,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
+      <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
       <c r="F7" s="14"/>
@@ -4344,7 +4344,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="11"/>
-      <c r="C8" s="12"/>
+      <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
@@ -4360,7 +4360,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="12"/>
+      <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
@@ -4376,7 +4376,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
+      <c r="C10" s="11"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
@@ -4392,7 +4392,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
+      <c r="C11" s="11"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
@@ -4408,7 +4408,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
+      <c r="C12" s="11"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
@@ -4424,7 +4424,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
+      <c r="C13" s="11"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
@@ -4440,7 +4440,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
+      <c r="C14" s="11"/>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
@@ -4456,7 +4456,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
+      <c r="C15" s="11"/>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
@@ -4472,7 +4472,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="11"/>
-      <c r="C16" s="12"/>
+      <c r="C16" s="11"/>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
@@ -4488,7 +4488,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="11"/>
-      <c r="C17" s="12"/>
+      <c r="C17" s="11"/>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
@@ -4504,7 +4504,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="11"/>
-      <c r="C18" s="12"/>
+      <c r="C18" s="11"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
@@ -4520,7 +4520,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="11"/>
-      <c r="C19" s="12"/>
+      <c r="C19" s="11"/>
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
@@ -4536,7 +4536,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="11"/>
-      <c r="C20" s="12"/>
+      <c r="C20" s="11"/>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
@@ -4552,7 +4552,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="11"/>
-      <c r="C21" s="12"/>
+      <c r="C21" s="11"/>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
@@ -4568,7 +4568,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="11"/>
-      <c r="C22" s="12"/>
+      <c r="C22" s="11"/>
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
@@ -4584,7 +4584,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="11"/>
-      <c r="C23" s="12"/>
+      <c r="C23" s="11"/>
       <c r="D23" s="11"/>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
@@ -4600,7 +4600,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="11"/>
-      <c r="C24" s="12"/>
+      <c r="C24" s="11"/>
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
@@ -4616,7 +4616,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="11"/>
-      <c r="C25" s="12"/>
+      <c r="C25" s="11"/>
       <c r="D25" s="11"/>
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
@@ -4632,7 +4632,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="11"/>
-      <c r="C26" s="12"/>
+      <c r="C26" s="11"/>
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
@@ -4648,7 +4648,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="11"/>
-      <c r="C27" s="12"/>
+      <c r="C27" s="11"/>
       <c r="D27" s="11"/>
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
@@ -4664,7 +4664,7 @@
         <v>25</v>
       </c>
       <c r="B28" s="11"/>
-      <c r="C28" s="12"/>
+      <c r="C28" s="11"/>
       <c r="D28" s="11"/>
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
@@ -4680,7 +4680,7 @@
         <v>26</v>
       </c>
       <c r="B29" s="11"/>
-      <c r="C29" s="12"/>
+      <c r="C29" s="11"/>
       <c r="D29" s="11"/>
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
@@ -4696,7 +4696,7 @@
         <v>27</v>
       </c>
       <c r="B30" s="11"/>
-      <c r="C30" s="12"/>
+      <c r="C30" s="11"/>
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
       <c r="F30" s="11"/>
@@ -4712,7 +4712,7 @@
         <v>28</v>
       </c>
       <c r="B31" s="11"/>
-      <c r="C31" s="12"/>
+      <c r="C31" s="11"/>
       <c r="D31" s="11"/>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
@@ -4728,7 +4728,7 @@
         <v>29</v>
       </c>
       <c r="B32" s="11"/>
-      <c r="C32" s="12"/>
+      <c r="C32" s="11"/>
       <c r="D32" s="11"/>
       <c r="E32" s="11"/>
       <c r="F32" s="11"/>
@@ -4744,7 +4744,7 @@
         <v>30</v>
       </c>
       <c r="B33" s="11"/>
-      <c r="C33" s="12"/>
+      <c r="C33" s="11"/>
       <c r="D33" s="11"/>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
@@ -4760,7 +4760,7 @@
         <v>31</v>
       </c>
       <c r="B34" s="11"/>
-      <c r="C34" s="12"/>
+      <c r="C34" s="11"/>
       <c r="D34" s="11"/>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
@@ -4776,7 +4776,7 @@
         <v>32</v>
       </c>
       <c r="B35" s="11"/>
-      <c r="C35" s="12"/>
+      <c r="C35" s="11"/>
       <c r="D35" s="11"/>
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
@@ -4792,7 +4792,7 @@
         <v>33</v>
       </c>
       <c r="B36" s="11"/>
-      <c r="C36" s="12"/>
+      <c r="C36" s="11"/>
       <c r="D36" s="11"/>
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
@@ -4808,7 +4808,7 @@
         <v>34</v>
       </c>
       <c r="B37" s="11"/>
-      <c r="C37" s="12"/>
+      <c r="C37" s="11"/>
       <c r="D37" s="11"/>
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
@@ -4824,7 +4824,7 @@
         <v>35</v>
       </c>
       <c r="B38" s="11"/>
-      <c r="C38" s="12"/>
+      <c r="C38" s="11"/>
       <c r="D38" s="11"/>
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
@@ -4840,7 +4840,7 @@
         <v>36</v>
       </c>
       <c r="B39" s="11"/>
-      <c r="C39" s="12"/>
+      <c r="C39" s="11"/>
       <c r="D39" s="11"/>
       <c r="E39" s="11"/>
       <c r="F39" s="11"/>
@@ -4856,7 +4856,7 @@
         <v>37</v>
       </c>
       <c r="B40" s="11"/>
-      <c r="C40" s="12"/>
+      <c r="C40" s="11"/>
       <c r="D40" s="11"/>
       <c r="E40" s="11"/>
       <c r="F40" s="11"/>
@@ -4872,7 +4872,7 @@
         <v>38</v>
       </c>
       <c r="B41" s="11"/>
-      <c r="C41" s="12"/>
+      <c r="C41" s="11"/>
       <c r="D41" s="11"/>
       <c r="E41" s="11"/>
       <c r="F41" s="11"/>
@@ -4888,7 +4888,7 @@
         <v>39</v>
       </c>
       <c r="B42" s="11"/>
-      <c r="C42" s="12"/>
+      <c r="C42" s="11"/>
       <c r="D42" s="11"/>
       <c r="E42" s="11"/>
       <c r="F42" s="11"/>
@@ -4904,7 +4904,7 @@
         <v>40</v>
       </c>
       <c r="B43" s="11"/>
-      <c r="C43" s="12"/>
+      <c r="C43" s="11"/>
       <c r="D43" s="11"/>
       <c r="E43" s="11"/>
       <c r="F43" s="11"/>
@@ -4920,7 +4920,7 @@
         <v>41</v>
       </c>
       <c r="B44" s="11"/>
-      <c r="C44" s="12"/>
+      <c r="C44" s="11"/>
       <c r="D44" s="11"/>
       <c r="E44" s="11"/>
       <c r="F44" s="11"/>
@@ -4936,7 +4936,7 @@
         <v>42</v>
       </c>
       <c r="B45" s="11"/>
-      <c r="C45" s="12"/>
+      <c r="C45" s="11"/>
       <c r="D45" s="11"/>
       <c r="E45" s="11"/>
       <c r="F45" s="11"/>
@@ -4952,7 +4952,7 @@
         <v>43</v>
       </c>
       <c r="B46" s="11"/>
-      <c r="C46" s="12"/>
+      <c r="C46" s="11"/>
       <c r="D46" s="11"/>
       <c r="E46" s="11"/>
       <c r="F46" s="11"/>
@@ -4968,7 +4968,7 @@
         <v>44</v>
       </c>
       <c r="B47" s="11"/>
-      <c r="C47" s="12"/>
+      <c r="C47" s="11"/>
       <c r="D47" s="11"/>
       <c r="E47" s="11"/>
       <c r="F47" s="11"/>
@@ -4984,7 +4984,7 @@
         <v>45</v>
       </c>
       <c r="B48" s="11"/>
-      <c r="C48" s="12"/>
+      <c r="C48" s="11"/>
       <c r="D48" s="11"/>
       <c r="E48" s="11"/>
       <c r="F48" s="11"/>
@@ -5000,7 +5000,7 @@
         <v>46</v>
       </c>
       <c r="B49" s="11"/>
-      <c r="C49" s="12"/>
+      <c r="C49" s="11"/>
       <c r="D49" s="11"/>
       <c r="E49" s="11"/>
       <c r="F49" s="11"/>
@@ -5016,7 +5016,7 @@
         <v>47</v>
       </c>
       <c r="B50" s="11"/>
-      <c r="C50" s="12"/>
+      <c r="C50" s="11"/>
       <c r="D50" s="11"/>
       <c r="E50" s="11"/>
       <c r="F50" s="11"/>
@@ -5032,7 +5032,7 @@
         <v>48</v>
       </c>
       <c r="B51" s="11"/>
-      <c r="C51" s="12"/>
+      <c r="C51" s="11"/>
       <c r="D51" s="11"/>
       <c r="E51" s="11"/>
       <c r="F51" s="11"/>
@@ -5048,7 +5048,7 @@
         <v>49</v>
       </c>
       <c r="B52" s="11"/>
-      <c r="C52" s="12"/>
+      <c r="C52" s="11"/>
       <c r="D52" s="11"/>
       <c r="E52" s="11"/>
       <c r="F52" s="11"/>
@@ -5064,7 +5064,7 @@
         <v>50</v>
       </c>
       <c r="B53" s="11"/>
-      <c r="C53" s="12"/>
+      <c r="C53" s="11"/>
       <c r="D53" s="11"/>
       <c r="E53" s="11"/>
       <c r="F53" s="11"/>
@@ -5080,7 +5080,7 @@
         <v>51</v>
       </c>
       <c r="B54" s="11"/>
-      <c r="C54" s="12"/>
+      <c r="C54" s="11"/>
       <c r="D54" s="11"/>
       <c r="E54" s="11"/>
       <c r="F54" s="11"/>
@@ -5096,7 +5096,7 @@
         <v>52</v>
       </c>
       <c r="B55" s="11"/>
-      <c r="C55" s="12"/>
+      <c r="C55" s="11"/>
       <c r="D55" s="11"/>
       <c r="E55" s="11"/>
       <c r="F55" s="11"/>
@@ -5112,7 +5112,7 @@
         <v>53</v>
       </c>
       <c r="B56" s="11"/>
-      <c r="C56" s="12"/>
+      <c r="C56" s="11"/>
       <c r="D56" s="11"/>
       <c r="E56" s="11"/>
       <c r="F56" s="11"/>
@@ -5128,7 +5128,7 @@
         <v>54</v>
       </c>
       <c r="B57" s="11"/>
-      <c r="C57" s="12"/>
+      <c r="C57" s="11"/>
       <c r="D57" s="11"/>
       <c r="E57" s="11"/>
       <c r="F57" s="11"/>
@@ -5144,7 +5144,7 @@
         <v>55</v>
       </c>
       <c r="B58" s="11"/>
-      <c r="C58" s="12"/>
+      <c r="C58" s="11"/>
       <c r="D58" s="11"/>
       <c r="E58" s="11"/>
       <c r="F58" s="11"/>
@@ -5160,7 +5160,7 @@
         <v>56</v>
       </c>
       <c r="B59" s="11"/>
-      <c r="C59" s="12"/>
+      <c r="C59" s="11"/>
       <c r="D59" s="11"/>
       <c r="E59" s="11"/>
       <c r="F59" s="11"/>
@@ -5176,7 +5176,7 @@
         <v>57</v>
       </c>
       <c r="B60" s="11"/>
-      <c r="C60" s="12"/>
+      <c r="C60" s="11"/>
       <c r="D60" s="11"/>
       <c r="E60" s="11"/>
       <c r="F60" s="11"/>
@@ -5192,7 +5192,7 @@
         <v>58</v>
       </c>
       <c r="B61" s="11"/>
-      <c r="C61" s="12"/>
+      <c r="C61" s="11"/>
       <c r="D61" s="11"/>
       <c r="E61" s="11"/>
       <c r="F61" s="11"/>
@@ -5208,7 +5208,7 @@
         <v>59</v>
       </c>
       <c r="B62" s="11"/>
-      <c r="C62" s="12"/>
+      <c r="C62" s="11"/>
       <c r="D62" s="11"/>
       <c r="E62" s="11"/>
       <c r="F62" s="11"/>
@@ -5224,7 +5224,7 @@
         <v>60</v>
       </c>
       <c r="B63" s="11"/>
-      <c r="C63" s="12"/>
+      <c r="C63" s="11"/>
       <c r="D63" s="11"/>
       <c r="E63" s="11"/>
       <c r="F63" s="11"/>
@@ -5240,7 +5240,7 @@
         <v>61</v>
       </c>
       <c r="B64" s="11"/>
-      <c r="C64" s="12"/>
+      <c r="C64" s="11"/>
       <c r="D64" s="11"/>
       <c r="E64" s="11"/>
       <c r="F64" s="11"/>
@@ -5256,7 +5256,7 @@
         <v>62</v>
       </c>
       <c r="B65" s="11"/>
-      <c r="C65" s="12"/>
+      <c r="C65" s="11"/>
       <c r="D65" s="11"/>
       <c r="E65" s="11"/>
       <c r="F65" s="11"/>
@@ -5272,7 +5272,7 @@
         <v>63</v>
       </c>
       <c r="B66" s="11"/>
-      <c r="C66" s="12"/>
+      <c r="C66" s="11"/>
       <c r="D66" s="11"/>
       <c r="E66" s="11"/>
       <c r="F66" s="11"/>
@@ -5288,7 +5288,7 @@
         <v>64</v>
       </c>
       <c r="B67" s="11"/>
-      <c r="C67" s="12"/>
+      <c r="C67" s="11"/>
       <c r="D67" s="11"/>
       <c r="E67" s="11"/>
       <c r="F67" s="11"/>
@@ -5304,7 +5304,7 @@
         <v>65</v>
       </c>
       <c r="B68" s="11"/>
-      <c r="C68" s="12"/>
+      <c r="C68" s="11"/>
       <c r="D68" s="11"/>
       <c r="E68" s="11"/>
       <c r="F68" s="11"/>
@@ -5320,7 +5320,7 @@
         <v>66</v>
       </c>
       <c r="B69" s="11"/>
-      <c r="C69" s="12"/>
+      <c r="C69" s="11"/>
       <c r="D69" s="11"/>
       <c r="E69" s="11"/>
       <c r="F69" s="11"/>
@@ -5336,7 +5336,7 @@
         <v>67</v>
       </c>
       <c r="B70" s="11"/>
-      <c r="C70" s="12"/>
+      <c r="C70" s="11"/>
       <c r="D70" s="11"/>
       <c r="E70" s="11"/>
       <c r="F70" s="11"/>
@@ -5352,7 +5352,7 @@
         <v>68</v>
       </c>
       <c r="B71" s="11"/>
-      <c r="C71" s="12"/>
+      <c r="C71" s="11"/>
       <c r="D71" s="11"/>
       <c r="E71" s="11"/>
       <c r="F71" s="11"/>
@@ -5368,7 +5368,7 @@
         <v>69</v>
       </c>
       <c r="B72" s="11"/>
-      <c r="C72" s="12"/>
+      <c r="C72" s="11"/>
       <c r="D72" s="11"/>
       <c r="E72" s="11"/>
       <c r="F72" s="11"/>
@@ -5384,7 +5384,7 @@
         <v>70</v>
       </c>
       <c r="B73" s="11"/>
-      <c r="C73" s="12"/>
+      <c r="C73" s="11"/>
       <c r="D73" s="11"/>
       <c r="E73" s="11"/>
       <c r="F73" s="11"/>
@@ -5400,7 +5400,7 @@
         <v>71</v>
       </c>
       <c r="B74" s="11"/>
-      <c r="C74" s="12"/>
+      <c r="C74" s="11"/>
       <c r="D74" s="11"/>
       <c r="E74" s="11"/>
       <c r="F74" s="11"/>
@@ -5416,7 +5416,7 @@
         <v>72</v>
       </c>
       <c r="B75" s="11"/>
-      <c r="C75" s="12"/>
+      <c r="C75" s="11"/>
       <c r="D75" s="11"/>
       <c r="E75" s="11"/>
       <c r="F75" s="11"/>
@@ -5432,7 +5432,7 @@
         <v>73</v>
       </c>
       <c r="B76" s="11"/>
-      <c r="C76" s="12"/>
+      <c r="C76" s="11"/>
       <c r="D76" s="11"/>
       <c r="E76" s="11"/>
       <c r="F76" s="11"/>
@@ -5448,7 +5448,7 @@
         <v>74</v>
       </c>
       <c r="B77" s="11"/>
-      <c r="C77" s="12"/>
+      <c r="C77" s="11"/>
       <c r="D77" s="11"/>
       <c r="E77" s="11"/>
       <c r="F77" s="11"/>
@@ -5464,7 +5464,7 @@
         <v>75</v>
       </c>
       <c r="B78" s="11"/>
-      <c r="C78" s="12"/>
+      <c r="C78" s="11"/>
       <c r="D78" s="11"/>
       <c r="E78" s="11"/>
       <c r="F78" s="11"/>
@@ -5480,7 +5480,7 @@
         <v>76</v>
       </c>
       <c r="B79" s="11"/>
-      <c r="C79" s="12"/>
+      <c r="C79" s="11"/>
       <c r="D79" s="11"/>
       <c r="E79" s="11"/>
       <c r="F79" s="11"/>
@@ -5496,7 +5496,7 @@
         <v>77</v>
       </c>
       <c r="B80" s="11"/>
-      <c r="C80" s="12"/>
+      <c r="C80" s="11"/>
       <c r="D80" s="11"/>
       <c r="E80" s="11"/>
       <c r="F80" s="11"/>
@@ -5512,7 +5512,7 @@
         <v>78</v>
       </c>
       <c r="B81" s="11"/>
-      <c r="C81" s="12"/>
+      <c r="C81" s="11"/>
       <c r="D81" s="11"/>
       <c r="E81" s="11"/>
       <c r="F81" s="11"/>
@@ -5528,7 +5528,7 @@
         <v>79</v>
       </c>
       <c r="B82" s="11"/>
-      <c r="C82" s="12"/>
+      <c r="C82" s="11"/>
       <c r="D82" s="11"/>
       <c r="E82" s="11"/>
       <c r="F82" s="11"/>
@@ -5544,7 +5544,7 @@
         <v>80</v>
       </c>
       <c r="B83" s="11"/>
-      <c r="C83" s="12"/>
+      <c r="C83" s="11"/>
       <c r="D83" s="11"/>
       <c r="E83" s="11"/>
       <c r="F83" s="11"/>
@@ -5560,7 +5560,7 @@
         <v>81</v>
       </c>
       <c r="B84" s="11"/>
-      <c r="C84" s="12"/>
+      <c r="C84" s="11"/>
       <c r="D84" s="11"/>
       <c r="E84" s="11"/>
       <c r="F84" s="11"/>
@@ -5576,7 +5576,7 @@
         <v>82</v>
       </c>
       <c r="B85" s="11"/>
-      <c r="C85" s="12"/>
+      <c r="C85" s="11"/>
       <c r="D85" s="11"/>
       <c r="E85" s="11"/>
       <c r="F85" s="11"/>
@@ -5592,7 +5592,7 @@
         <v>83</v>
       </c>
       <c r="B86" s="11"/>
-      <c r="C86" s="12"/>
+      <c r="C86" s="11"/>
       <c r="D86" s="11"/>
       <c r="E86" s="11"/>
       <c r="F86" s="11"/>
@@ -5608,7 +5608,7 @@
         <v>84</v>
       </c>
       <c r="B87" s="11"/>
-      <c r="C87" s="12"/>
+      <c r="C87" s="11"/>
       <c r="D87" s="11"/>
       <c r="E87" s="11"/>
       <c r="F87" s="11"/>
@@ -5624,7 +5624,7 @@
         <v>85</v>
       </c>
       <c r="B88" s="11"/>
-      <c r="C88" s="12"/>
+      <c r="C88" s="11"/>
       <c r="D88" s="11"/>
       <c r="E88" s="11"/>
       <c r="F88" s="11"/>
@@ -5640,7 +5640,7 @@
         <v>86</v>
       </c>
       <c r="B89" s="11"/>
-      <c r="C89" s="12"/>
+      <c r="C89" s="11"/>
       <c r="D89" s="11"/>
       <c r="E89" s="11"/>
       <c r="F89" s="11"/>
@@ -5656,7 +5656,7 @@
         <v>87</v>
       </c>
       <c r="B90" s="11"/>
-      <c r="C90" s="12"/>
+      <c r="C90" s="11"/>
       <c r="D90" s="11"/>
       <c r="E90" s="11"/>
       <c r="F90" s="11"/>
@@ -5672,7 +5672,7 @@
         <v>88</v>
       </c>
       <c r="B91" s="11"/>
-      <c r="C91" s="12"/>
+      <c r="C91" s="11"/>
       <c r="D91" s="11"/>
       <c r="E91" s="11"/>
       <c r="F91" s="11"/>
@@ -5688,7 +5688,7 @@
         <v>89</v>
       </c>
       <c r="B92" s="11"/>
-      <c r="C92" s="12"/>
+      <c r="C92" s="11"/>
       <c r="D92" s="11"/>
       <c r="E92" s="11"/>
       <c r="F92" s="11"/>
@@ -5704,7 +5704,7 @@
         <v>90</v>
       </c>
       <c r="B93" s="11"/>
-      <c r="C93" s="12"/>
+      <c r="C93" s="11"/>
       <c r="D93" s="11"/>
       <c r="E93" s="11"/>
       <c r="F93" s="11"/>
@@ -5720,7 +5720,7 @@
         <v>91</v>
       </c>
       <c r="B94" s="11"/>
-      <c r="C94" s="12"/>
+      <c r="C94" s="11"/>
       <c r="D94" s="11"/>
       <c r="E94" s="11"/>
       <c r="F94" s="11"/>
@@ -5736,7 +5736,7 @@
         <v>92</v>
       </c>
       <c r="B95" s="11"/>
-      <c r="C95" s="12"/>
+      <c r="C95" s="11"/>
       <c r="D95" s="11"/>
       <c r="E95" s="11"/>
       <c r="F95" s="11"/>
@@ -5752,7 +5752,7 @@
         <v>93</v>
       </c>
       <c r="B96" s="11"/>
-      <c r="C96" s="12"/>
+      <c r="C96" s="11"/>
       <c r="D96" s="11"/>
       <c r="E96" s="11"/>
       <c r="F96" s="11"/>
@@ -5768,7 +5768,7 @@
         <v>94</v>
       </c>
       <c r="B97" s="11"/>
-      <c r="C97" s="12"/>
+      <c r="C97" s="11"/>
       <c r="D97" s="11"/>
       <c r="E97" s="11"/>
       <c r="F97" s="11"/>
@@ -5784,7 +5784,7 @@
         <v>95</v>
       </c>
       <c r="B98" s="11"/>
-      <c r="C98" s="12"/>
+      <c r="C98" s="11"/>
       <c r="D98" s="11"/>
       <c r="E98" s="11"/>
       <c r="F98" s="11"/>
@@ -5800,7 +5800,7 @@
         <v>96</v>
       </c>
       <c r="B99" s="11"/>
-      <c r="C99" s="12"/>
+      <c r="C99" s="11"/>
       <c r="D99" s="11"/>
       <c r="E99" s="11"/>
       <c r="F99" s="11"/>
@@ -5816,7 +5816,7 @@
         <v>97</v>
       </c>
       <c r="B100" s="11"/>
-      <c r="C100" s="12"/>
+      <c r="C100" s="11"/>
       <c r="D100" s="11"/>
       <c r="E100" s="11"/>
       <c r="F100" s="11"/>
@@ -5832,7 +5832,7 @@
         <v>98</v>
       </c>
       <c r="B101" s="11"/>
-      <c r="C101" s="12"/>
+      <c r="C101" s="11"/>
       <c r="D101" s="11"/>
       <c r="E101" s="11"/>
       <c r="F101" s="11"/>
@@ -5848,7 +5848,7 @@
         <v>99</v>
       </c>
       <c r="B102" s="11"/>
-      <c r="C102" s="12"/>
+      <c r="C102" s="11"/>
       <c r="D102" s="11"/>
       <c r="E102" s="11"/>
       <c r="F102" s="11"/>
@@ -5864,7 +5864,7 @@
         <v>100</v>
       </c>
       <c r="B103" s="11"/>
-      <c r="C103" s="12"/>
+      <c r="C103" s="11"/>
       <c r="D103" s="11"/>
       <c r="E103" s="11"/>
       <c r="F103" s="11"/>
@@ -5880,7 +5880,7 @@
         <v>101</v>
       </c>
       <c r="B104" s="11"/>
-      <c r="C104" s="12"/>
+      <c r="C104" s="11"/>
       <c r="D104" s="11"/>
       <c r="E104" s="11"/>
       <c r="F104" s="11"/>
@@ -5896,7 +5896,7 @@
         <v>102</v>
       </c>
       <c r="B105" s="11"/>
-      <c r="C105" s="12"/>
+      <c r="C105" s="11"/>
       <c r="D105" s="11"/>
       <c r="E105" s="11"/>
       <c r="F105" s="11"/>
@@ -5912,7 +5912,7 @@
         <v>103</v>
       </c>
       <c r="B106" s="11"/>
-      <c r="C106" s="12"/>
+      <c r="C106" s="11"/>
       <c r="D106" s="11"/>
       <c r="E106" s="11"/>
       <c r="F106" s="11"/>
@@ -5928,7 +5928,7 @@
         <v>104</v>
       </c>
       <c r="B107" s="11"/>
-      <c r="C107" s="12"/>
+      <c r="C107" s="11"/>
       <c r="D107" s="11"/>
       <c r="E107" s="11"/>
       <c r="F107" s="11"/>
@@ -5944,7 +5944,7 @@
         <v>105</v>
       </c>
       <c r="B108" s="11"/>
-      <c r="C108" s="12"/>
+      <c r="C108" s="11"/>
       <c r="D108" s="11"/>
       <c r="E108" s="11"/>
       <c r="F108" s="11"/>
@@ -5960,7 +5960,7 @@
         <v>106</v>
       </c>
       <c r="B109" s="11"/>
-      <c r="C109" s="12"/>
+      <c r="C109" s="11"/>
       <c r="D109" s="11"/>
       <c r="E109" s="11"/>
       <c r="F109" s="11"/>
@@ -5976,7 +5976,7 @@
         <v>107</v>
       </c>
       <c r="B110" s="11"/>
-      <c r="C110" s="12"/>
+      <c r="C110" s="11"/>
       <c r="D110" s="11"/>
       <c r="E110" s="11"/>
       <c r="F110" s="11"/>
@@ -5992,7 +5992,7 @@
         <v>108</v>
       </c>
       <c r="B111" s="11"/>
-      <c r="C111" s="12"/>
+      <c r="C111" s="11"/>
       <c r="D111" s="11"/>
       <c r="E111" s="11"/>
       <c r="F111" s="11"/>
@@ -6008,7 +6008,7 @@
         <v>109</v>
       </c>
       <c r="B112" s="11"/>
-      <c r="C112" s="12"/>
+      <c r="C112" s="11"/>
       <c r="D112" s="11"/>
       <c r="E112" s="11"/>
       <c r="F112" s="11"/>
@@ -6024,7 +6024,7 @@
         <v>110</v>
       </c>
       <c r="B113" s="11"/>
-      <c r="C113" s="12"/>
+      <c r="C113" s="11"/>
       <c r="D113" s="11"/>
       <c r="E113" s="11"/>
       <c r="F113" s="11"/>
@@ -6040,7 +6040,7 @@
         <v>111</v>
       </c>
       <c r="B114" s="11"/>
-      <c r="C114" s="12"/>
+      <c r="C114" s="11"/>
       <c r="D114" s="11"/>
       <c r="E114" s="11"/>
       <c r="F114" s="11"/>
@@ -6056,7 +6056,7 @@
         <v>112</v>
       </c>
       <c r="B115" s="11"/>
-      <c r="C115" s="12"/>
+      <c r="C115" s="11"/>
       <c r="D115" s="11"/>
       <c r="E115" s="11"/>
       <c r="F115" s="11"/>
@@ -6072,7 +6072,7 @@
         <v>113</v>
       </c>
       <c r="B116" s="11"/>
-      <c r="C116" s="12"/>
+      <c r="C116" s="11"/>
       <c r="D116" s="11"/>
       <c r="E116" s="11"/>
       <c r="F116" s="11"/>
@@ -6088,7 +6088,7 @@
         <v>114</v>
       </c>
       <c r="B117" s="11"/>
-      <c r="C117" s="12"/>
+      <c r="C117" s="11"/>
       <c r="D117" s="11"/>
       <c r="E117" s="11"/>
       <c r="F117" s="11"/>
@@ -6104,7 +6104,7 @@
         <v>115</v>
       </c>
       <c r="B118" s="11"/>
-      <c r="C118" s="12"/>
+      <c r="C118" s="11"/>
       <c r="D118" s="11"/>
       <c r="E118" s="11"/>
       <c r="F118" s="11"/>
@@ -6120,7 +6120,7 @@
         <v>116</v>
       </c>
       <c r="B119" s="11"/>
-      <c r="C119" s="12"/>
+      <c r="C119" s="11"/>
       <c r="D119" s="11"/>
       <c r="E119" s="11"/>
       <c r="F119" s="11"/>
@@ -6136,7 +6136,7 @@
         <v>117</v>
       </c>
       <c r="B120" s="11"/>
-      <c r="C120" s="12"/>
+      <c r="C120" s="11"/>
       <c r="D120" s="11"/>
       <c r="E120" s="11"/>
       <c r="F120" s="11"/>
@@ -6152,7 +6152,7 @@
         <v>118</v>
       </c>
       <c r="B121" s="11"/>
-      <c r="C121" s="12"/>
+      <c r="C121" s="11"/>
       <c r="D121" s="11"/>
       <c r="E121" s="11"/>
       <c r="F121" s="11"/>
@@ -6168,7 +6168,7 @@
         <v>119</v>
       </c>
       <c r="B122" s="11"/>
-      <c r="C122" s="12"/>
+      <c r="C122" s="11"/>
       <c r="D122" s="11"/>
       <c r="E122" s="11"/>
       <c r="F122" s="11"/>
@@ -6184,7 +6184,7 @@
         <v>120</v>
       </c>
       <c r="B123" s="11"/>
-      <c r="C123" s="12"/>
+      <c r="C123" s="11"/>
       <c r="D123" s="11"/>
       <c r="E123" s="11"/>
       <c r="F123" s="11"/>
@@ -6200,7 +6200,7 @@
         <v>121</v>
       </c>
       <c r="B124" s="11"/>
-      <c r="C124" s="12"/>
+      <c r="C124" s="11"/>
       <c r="D124" s="11"/>
       <c r="E124" s="11"/>
       <c r="F124" s="11"/>
@@ -6216,7 +6216,7 @@
         <v>122</v>
       </c>
       <c r="B125" s="11"/>
-      <c r="C125" s="12"/>
+      <c r="C125" s="11"/>
       <c r="D125" s="11"/>
       <c r="E125" s="11"/>
       <c r="F125" s="11"/>
@@ -6232,7 +6232,7 @@
         <v>123</v>
       </c>
       <c r="B126" s="11"/>
-      <c r="C126" s="12"/>
+      <c r="C126" s="11"/>
       <c r="D126" s="11"/>
       <c r="E126" s="11"/>
       <c r="F126" s="11"/>
@@ -6248,7 +6248,7 @@
         <v>124</v>
       </c>
       <c r="B127" s="11"/>
-      <c r="C127" s="12"/>
+      <c r="C127" s="11"/>
       <c r="D127" s="11"/>
       <c r="E127" s="11"/>
       <c r="F127" s="11"/>
@@ -6264,7 +6264,7 @@
         <v>125</v>
       </c>
       <c r="B128" s="11"/>
-      <c r="C128" s="12"/>
+      <c r="C128" s="11"/>
       <c r="D128" s="11"/>
       <c r="E128" s="11"/>
       <c r="F128" s="11"/>
@@ -6280,7 +6280,7 @@
         <v>126</v>
       </c>
       <c r="B129" s="11"/>
-      <c r="C129" s="12"/>
+      <c r="C129" s="11"/>
       <c r="D129" s="11"/>
       <c r="E129" s="11"/>
       <c r="F129" s="11"/>
@@ -6296,7 +6296,7 @@
         <v>127</v>
       </c>
       <c r="B130" s="11"/>
-      <c r="C130" s="12"/>
+      <c r="C130" s="11"/>
       <c r="D130" s="11"/>
       <c r="E130" s="11"/>
       <c r="F130" s="11"/>
@@ -6312,7 +6312,7 @@
         <v>128</v>
       </c>
       <c r="B131" s="11"/>
-      <c r="C131" s="12"/>
+      <c r="C131" s="11"/>
       <c r="D131" s="11"/>
       <c r="E131" s="11"/>
       <c r="F131" s="11"/>
@@ -6328,7 +6328,7 @@
         <v>129</v>
       </c>
       <c r="B132" s="11"/>
-      <c r="C132" s="12"/>
+      <c r="C132" s="11"/>
       <c r="D132" s="11"/>
       <c r="E132" s="11"/>
       <c r="F132" s="11"/>
@@ -6344,7 +6344,7 @@
         <v>130</v>
       </c>
       <c r="B133" s="11"/>
-      <c r="C133" s="12"/>
+      <c r="C133" s="11"/>
       <c r="D133" s="11"/>
       <c r="E133" s="11"/>
       <c r="F133" s="11"/>
@@ -6360,7 +6360,7 @@
         <v>131</v>
       </c>
       <c r="B134" s="11"/>
-      <c r="C134" s="12"/>
+      <c r="C134" s="11"/>
       <c r="D134" s="11"/>
       <c r="E134" s="11"/>
       <c r="F134" s="11"/>
@@ -6376,7 +6376,7 @@
         <v>132</v>
       </c>
       <c r="B135" s="11"/>
-      <c r="C135" s="12"/>
+      <c r="C135" s="11"/>
       <c r="D135" s="11"/>
       <c r="E135" s="11"/>
       <c r="F135" s="11"/>
@@ -6392,7 +6392,7 @@
         <v>133</v>
       </c>
       <c r="B136" s="11"/>
-      <c r="C136" s="12"/>
+      <c r="C136" s="11"/>
       <c r="D136" s="11"/>
       <c r="E136" s="11"/>
       <c r="F136" s="11"/>
@@ -6408,7 +6408,7 @@
         <v>134</v>
       </c>
       <c r="B137" s="11"/>
-      <c r="C137" s="12"/>
+      <c r="C137" s="11"/>
       <c r="D137" s="11"/>
       <c r="E137" s="11"/>
       <c r="F137" s="11"/>
@@ -6424,7 +6424,7 @@
         <v>135</v>
       </c>
       <c r="B138" s="11"/>
-      <c r="C138" s="12"/>
+      <c r="C138" s="11"/>
       <c r="D138" s="11"/>
       <c r="E138" s="11"/>
       <c r="F138" s="11"/>
@@ -6440,7 +6440,7 @@
         <v>136</v>
       </c>
       <c r="B139" s="11"/>
-      <c r="C139" s="12"/>
+      <c r="C139" s="11"/>
       <c r="D139" s="11"/>
       <c r="E139" s="11"/>
       <c r="F139" s="11"/>
@@ -6456,7 +6456,7 @@
         <v>137</v>
       </c>
       <c r="B140" s="11"/>
-      <c r="C140" s="12"/>
+      <c r="C140" s="11"/>
       <c r="D140" s="11"/>
       <c r="E140" s="11"/>
       <c r="F140" s="11"/>
@@ -6472,7 +6472,7 @@
         <v>138</v>
       </c>
       <c r="B141" s="11"/>
-      <c r="C141" s="12"/>
+      <c r="C141" s="11"/>
       <c r="D141" s="11"/>
       <c r="E141" s="11"/>
       <c r="F141" s="11"/>
@@ -6488,7 +6488,7 @@
         <v>139</v>
       </c>
       <c r="B142" s="11"/>
-      <c r="C142" s="12"/>
+      <c r="C142" s="11"/>
       <c r="D142" s="11"/>
       <c r="E142" s="11"/>
       <c r="F142" s="11"/>
@@ -6504,7 +6504,7 @@
         <v>140</v>
       </c>
       <c r="B143" s="11"/>
-      <c r="C143" s="12"/>
+      <c r="C143" s="11"/>
       <c r="D143" s="11"/>
       <c r="E143" s="11"/>
       <c r="F143" s="11"/>
@@ -6520,7 +6520,7 @@
         <v>141</v>
       </c>
       <c r="B144" s="11"/>
-      <c r="C144" s="12"/>
+      <c r="C144" s="11"/>
       <c r="D144" s="11"/>
       <c r="E144" s="11"/>
       <c r="F144" s="11"/>
@@ -6536,7 +6536,7 @@
         <v>142</v>
       </c>
       <c r="B145" s="11"/>
-      <c r="C145" s="12"/>
+      <c r="C145" s="11"/>
       <c r="D145" s="11"/>
       <c r="E145" s="11"/>
       <c r="F145" s="11"/>
@@ -6552,7 +6552,7 @@
         <v>143</v>
       </c>
       <c r="B146" s="11"/>
-      <c r="C146" s="12"/>
+      <c r="C146" s="11"/>
       <c r="D146" s="11"/>
       <c r="E146" s="11"/>
       <c r="F146" s="11"/>
@@ -6568,7 +6568,7 @@
         <v>144</v>
       </c>
       <c r="B147" s="11"/>
-      <c r="C147" s="12"/>
+      <c r="C147" s="11"/>
       <c r="D147" s="11"/>
       <c r="E147" s="11"/>
       <c r="F147" s="11"/>
@@ -6584,7 +6584,7 @@
         <v>145</v>
       </c>
       <c r="B148" s="11"/>
-      <c r="C148" s="12"/>
+      <c r="C148" s="11"/>
       <c r="D148" s="11"/>
       <c r="E148" s="11"/>
       <c r="F148" s="11"/>
@@ -6600,7 +6600,7 @@
         <v>146</v>
       </c>
       <c r="B149" s="11"/>
-      <c r="C149" s="12"/>
+      <c r="C149" s="11"/>
       <c r="D149" s="11"/>
       <c r="E149" s="11"/>
       <c r="F149" s="11"/>
@@ -6616,7 +6616,7 @@
         <v>147</v>
       </c>
       <c r="B150" s="11"/>
-      <c r="C150" s="12"/>
+      <c r="C150" s="11"/>
       <c r="D150" s="11"/>
       <c r="E150" s="11"/>
       <c r="F150" s="11"/>
@@ -6632,7 +6632,7 @@
         <v>148</v>
       </c>
       <c r="B151" s="11"/>
-      <c r="C151" s="12"/>
+      <c r="C151" s="11"/>
       <c r="D151" s="11"/>
       <c r="E151" s="11"/>
       <c r="F151" s="11"/>
@@ -6648,7 +6648,7 @@
         <v>149</v>
       </c>
       <c r="B152" s="11"/>
-      <c r="C152" s="12"/>
+      <c r="C152" s="11"/>
       <c r="D152" s="11"/>
       <c r="E152" s="11"/>
       <c r="F152" s="11"/>
@@ -6664,7 +6664,7 @@
         <v>150</v>
       </c>
       <c r="B153" s="11"/>
-      <c r="C153" s="12"/>
+      <c r="C153" s="11"/>
       <c r="D153" s="11"/>
       <c r="E153" s="11"/>
       <c r="F153" s="11"/>
@@ -6680,7 +6680,7 @@
         <v>151</v>
       </c>
       <c r="B154" s="11"/>
-      <c r="C154" s="12"/>
+      <c r="C154" s="11"/>
       <c r="D154" s="11"/>
       <c r="E154" s="11"/>
       <c r="F154" s="11"/>
@@ -6696,7 +6696,7 @@
         <v>152</v>
       </c>
       <c r="B155" s="11"/>
-      <c r="C155" s="12"/>
+      <c r="C155" s="11"/>
       <c r="D155" s="11"/>
       <c r="E155" s="11"/>
       <c r="F155" s="11"/>
@@ -6712,7 +6712,7 @@
         <v>153</v>
       </c>
       <c r="B156" s="11"/>
-      <c r="C156" s="12"/>
+      <c r="C156" s="11"/>
       <c r="D156" s="11"/>
       <c r="E156" s="11"/>
       <c r="F156" s="11"/>
@@ -6728,7 +6728,7 @@
         <v>154</v>
       </c>
       <c r="B157" s="11"/>
-      <c r="C157" s="12"/>
+      <c r="C157" s="11"/>
       <c r="D157" s="11"/>
       <c r="E157" s="11"/>
       <c r="F157" s="11"/>
@@ -6744,7 +6744,7 @@
         <v>155</v>
       </c>
       <c r="B158" s="11"/>
-      <c r="C158" s="12"/>
+      <c r="C158" s="11"/>
       <c r="D158" s="11"/>
       <c r="E158" s="11"/>
       <c r="F158" s="11"/>
@@ -6760,7 +6760,7 @@
         <v>156</v>
       </c>
       <c r="B159" s="11"/>
-      <c r="C159" s="12"/>
+      <c r="C159" s="11"/>
       <c r="D159" s="11"/>
       <c r="E159" s="11"/>
       <c r="F159" s="11"/>
@@ -6776,7 +6776,7 @@
         <v>157</v>
       </c>
       <c r="B160" s="11"/>
-      <c r="C160" s="12"/>
+      <c r="C160" s="11"/>
       <c r="D160" s="11"/>
       <c r="E160" s="11"/>
       <c r="F160" s="11"/>
@@ -6792,7 +6792,7 @@
         <v>158</v>
       </c>
       <c r="B161" s="11"/>
-      <c r="C161" s="12"/>
+      <c r="C161" s="11"/>
       <c r="D161" s="11"/>
       <c r="E161" s="11"/>
       <c r="F161" s="11"/>
@@ -6808,7 +6808,7 @@
         <v>159</v>
       </c>
       <c r="B162" s="11"/>
-      <c r="C162" s="12"/>
+      <c r="C162" s="11"/>
       <c r="D162" s="11"/>
       <c r="E162" s="11"/>
       <c r="F162" s="11"/>
@@ -6824,7 +6824,7 @@
         <v>160</v>
       </c>
       <c r="B163" s="11"/>
-      <c r="C163" s="12"/>
+      <c r="C163" s="11"/>
       <c r="D163" s="11"/>
       <c r="E163" s="11"/>
       <c r="F163" s="11"/>
@@ -6840,7 +6840,7 @@
         <v>161</v>
       </c>
       <c r="B164" s="11"/>
-      <c r="C164" s="12"/>
+      <c r="C164" s="11"/>
       <c r="D164" s="11"/>
       <c r="E164" s="11"/>
       <c r="F164" s="11"/>
@@ -6856,7 +6856,7 @@
         <v>162</v>
       </c>
       <c r="B165" s="11"/>
-      <c r="C165" s="12"/>
+      <c r="C165" s="11"/>
       <c r="D165" s="11"/>
       <c r="E165" s="11"/>
       <c r="F165" s="11"/>
@@ -6872,7 +6872,7 @@
         <v>163</v>
       </c>
       <c r="B166" s="11"/>
-      <c r="C166" s="12"/>
+      <c r="C166" s="11"/>
       <c r="D166" s="11"/>
       <c r="E166" s="11"/>
       <c r="F166" s="11"/>
@@ -6888,7 +6888,7 @@
         <v>164</v>
       </c>
       <c r="B167" s="11"/>
-      <c r="C167" s="12"/>
+      <c r="C167" s="11"/>
       <c r="D167" s="11"/>
       <c r="E167" s="11"/>
       <c r="F167" s="11"/>
@@ -6904,7 +6904,7 @@
         <v>165</v>
       </c>
       <c r="B168" s="11"/>
-      <c r="C168" s="12"/>
+      <c r="C168" s="11"/>
       <c r="D168" s="11"/>
       <c r="E168" s="11"/>
       <c r="F168" s="11"/>
@@ -6920,7 +6920,7 @@
         <v>166</v>
       </c>
       <c r="B169" s="11"/>
-      <c r="C169" s="12"/>
+      <c r="C169" s="11"/>
       <c r="D169" s="11"/>
       <c r="E169" s="11"/>
       <c r="F169" s="11"/>
@@ -6936,7 +6936,7 @@
         <v>167</v>
       </c>
       <c r="B170" s="11"/>
-      <c r="C170" s="12"/>
+      <c r="C170" s="11"/>
       <c r="D170" s="11"/>
       <c r="E170" s="11"/>
       <c r="F170" s="11"/>
@@ -6952,7 +6952,7 @@
         <v>168</v>
       </c>
       <c r="B171" s="11"/>
-      <c r="C171" s="12"/>
+      <c r="C171" s="11"/>
       <c r="D171" s="11"/>
       <c r="E171" s="11"/>
       <c r="F171" s="11"/>
@@ -6968,7 +6968,7 @@
         <v>169</v>
       </c>
       <c r="B172" s="11"/>
-      <c r="C172" s="12"/>
+      <c r="C172" s="11"/>
       <c r="D172" s="11"/>
       <c r="E172" s="11"/>
       <c r="F172" s="11"/>
@@ -6984,7 +6984,7 @@
         <v>170</v>
       </c>
       <c r="B173" s="11"/>
-      <c r="C173" s="12"/>
+      <c r="C173" s="11"/>
       <c r="D173" s="11"/>
       <c r="E173" s="11"/>
       <c r="F173" s="11"/>
@@ -7000,7 +7000,7 @@
         <v>171</v>
       </c>
       <c r="B174" s="11"/>
-      <c r="C174" s="12"/>
+      <c r="C174" s="11"/>
       <c r="D174" s="11"/>
       <c r="E174" s="11"/>
       <c r="F174" s="11"/>
@@ -7016,7 +7016,7 @@
         <v>172</v>
       </c>
       <c r="B175" s="11"/>
-      <c r="C175" s="12"/>
+      <c r="C175" s="11"/>
       <c r="D175" s="11"/>
       <c r="E175" s="11"/>
       <c r="F175" s="11"/>
@@ -7032,7 +7032,7 @@
         <v>173</v>
       </c>
       <c r="B176" s="11"/>
-      <c r="C176" s="12"/>
+      <c r="C176" s="11"/>
       <c r="D176" s="11"/>
       <c r="E176" s="11"/>
       <c r="F176" s="11"/>
@@ -7048,7 +7048,7 @@
         <v>174</v>
       </c>
       <c r="B177" s="11"/>
-      <c r="C177" s="12"/>
+      <c r="C177" s="11"/>
       <c r="D177" s="11"/>
       <c r="E177" s="11"/>
       <c r="F177" s="11"/>
@@ -7064,7 +7064,7 @@
         <v>175</v>
       </c>
       <c r="B178" s="11"/>
-      <c r="C178" s="12"/>
+      <c r="C178" s="11"/>
       <c r="D178" s="11"/>
       <c r="E178" s="11"/>
       <c r="F178" s="11"/>
@@ -7080,7 +7080,7 @@
         <v>176</v>
       </c>
       <c r="B179" s="11"/>
-      <c r="C179" s="12"/>
+      <c r="C179" s="11"/>
       <c r="D179" s="11"/>
       <c r="E179" s="11"/>
       <c r="F179" s="11"/>
@@ -7096,7 +7096,7 @@
         <v>177</v>
       </c>
       <c r="B180" s="11"/>
-      <c r="C180" s="12"/>
+      <c r="C180" s="11"/>
       <c r="D180" s="11"/>
       <c r="E180" s="11"/>
       <c r="F180" s="11"/>
@@ -7112,7 +7112,7 @@
         <v>178</v>
       </c>
       <c r="B181" s="11"/>
-      <c r="C181" s="12"/>
+      <c r="C181" s="11"/>
       <c r="D181" s="11"/>
       <c r="E181" s="11"/>
       <c r="F181" s="11"/>
@@ -7128,7 +7128,7 @@
         <v>179</v>
       </c>
       <c r="B182" s="11"/>
-      <c r="C182" s="12"/>
+      <c r="C182" s="11"/>
       <c r="D182" s="11"/>
       <c r="E182" s="11"/>
       <c r="F182" s="11"/>
@@ -7144,7 +7144,7 @@
         <v>180</v>
       </c>
       <c r="B183" s="11"/>
-      <c r="C183" s="12"/>
+      <c r="C183" s="11"/>
       <c r="D183" s="11"/>
       <c r="E183" s="11"/>
       <c r="F183" s="11"/>
@@ -7160,7 +7160,7 @@
         <v>181</v>
       </c>
       <c r="B184" s="11"/>
-      <c r="C184" s="12"/>
+      <c r="C184" s="11"/>
       <c r="D184" s="11"/>
       <c r="E184" s="11"/>
       <c r="F184" s="11"/>
@@ -7176,7 +7176,7 @@
         <v>182</v>
       </c>
       <c r="B185" s="11"/>
-      <c r="C185" s="12"/>
+      <c r="C185" s="11"/>
       <c r="D185" s="11"/>
       <c r="E185" s="11"/>
       <c r="F185" s="11"/>
@@ -7192,7 +7192,7 @@
         <v>183</v>
       </c>
       <c r="B186" s="11"/>
-      <c r="C186" s="12"/>
+      <c r="C186" s="11"/>
       <c r="D186" s="11"/>
       <c r="E186" s="11"/>
       <c r="F186" s="11"/>
@@ -7208,7 +7208,7 @@
         <v>184</v>
       </c>
       <c r="B187" s="11"/>
-      <c r="C187" s="12"/>
+      <c r="C187" s="11"/>
       <c r="D187" s="11"/>
       <c r="E187" s="11"/>
       <c r="F187" s="11"/>
@@ -7224,7 +7224,7 @@
         <v>185</v>
       </c>
       <c r="B188" s="11"/>
-      <c r="C188" s="12"/>
+      <c r="C188" s="11"/>
       <c r="D188" s="11"/>
       <c r="E188" s="11"/>
       <c r="F188" s="11"/>
@@ -7240,7 +7240,7 @@
         <v>186</v>
       </c>
       <c r="B189" s="11"/>
-      <c r="C189" s="12"/>
+      <c r="C189" s="11"/>
       <c r="D189" s="11"/>
       <c r="E189" s="11"/>
       <c r="F189" s="11"/>
@@ -7256,7 +7256,7 @@
         <v>187</v>
       </c>
       <c r="B190" s="11"/>
-      <c r="C190" s="12"/>
+      <c r="C190" s="11"/>
       <c r="D190" s="11"/>
       <c r="E190" s="11"/>
       <c r="F190" s="11"/>
@@ -7272,7 +7272,7 @@
         <v>188</v>
       </c>
       <c r="B191" s="11"/>
-      <c r="C191" s="12"/>
+      <c r="C191" s="11"/>
       <c r="D191" s="11"/>
       <c r="E191" s="11"/>
       <c r="F191" s="11"/>
@@ -7288,7 +7288,7 @@
         <v>189</v>
       </c>
       <c r="B192" s="11"/>
-      <c r="C192" s="12"/>
+      <c r="C192" s="11"/>
       <c r="D192" s="11"/>
       <c r="E192" s="11"/>
       <c r="F192" s="11"/>
@@ -7304,7 +7304,7 @@
         <v>190</v>
       </c>
       <c r="B193" s="11"/>
-      <c r="C193" s="12"/>
+      <c r="C193" s="11"/>
       <c r="D193" s="11"/>
       <c r="E193" s="11"/>
       <c r="F193" s="11"/>
@@ -7320,7 +7320,7 @@
         <v>191</v>
       </c>
       <c r="B194" s="11"/>
-      <c r="C194" s="12"/>
+      <c r="C194" s="11"/>
       <c r="D194" s="11"/>
       <c r="E194" s="11"/>
       <c r="F194" s="11"/>
@@ -7336,7 +7336,7 @@
         <v>192</v>
       </c>
       <c r="B195" s="11"/>
-      <c r="C195" s="12"/>
+      <c r="C195" s="11"/>
       <c r="D195" s="11"/>
       <c r="E195" s="11"/>
       <c r="F195" s="11"/>
@@ -7352,7 +7352,7 @@
         <v>193</v>
       </c>
       <c r="B196" s="11"/>
-      <c r="C196" s="12"/>
+      <c r="C196" s="11"/>
       <c r="D196" s="11"/>
       <c r="E196" s="11"/>
       <c r="F196" s="11"/>
@@ -7368,7 +7368,7 @@
         <v>194</v>
       </c>
       <c r="B197" s="11"/>
-      <c r="C197" s="12"/>
+      <c r="C197" s="11"/>
       <c r="D197" s="11"/>
       <c r="E197" s="11"/>
       <c r="F197" s="11"/>
@@ -7384,7 +7384,7 @@
         <v>195</v>
       </c>
       <c r="B198" s="11"/>
-      <c r="C198" s="12"/>
+      <c r="C198" s="11"/>
       <c r="D198" s="11"/>
       <c r="E198" s="11"/>
       <c r="F198" s="11"/>
@@ -7400,7 +7400,7 @@
         <v>196</v>
       </c>
       <c r="B199" s="11"/>
-      <c r="C199" s="12"/>
+      <c r="C199" s="11"/>
       <c r="D199" s="11"/>
       <c r="E199" s="11"/>
       <c r="F199" s="11"/>
@@ -7416,7 +7416,7 @@
         <v>197</v>
       </c>
       <c r="B200" s="11"/>
-      <c r="C200" s="12"/>
+      <c r="C200" s="11"/>
       <c r="D200" s="11"/>
       <c r="E200" s="11"/>
       <c r="F200" s="11"/>
@@ -7432,7 +7432,7 @@
         <v>198</v>
       </c>
       <c r="B201" s="11"/>
-      <c r="C201" s="12"/>
+      <c r="C201" s="11"/>
       <c r="D201" s="11"/>
       <c r="E201" s="11"/>
       <c r="F201" s="11"/>
@@ -7448,7 +7448,7 @@
         <v>199</v>
       </c>
       <c r="B202" s="11"/>
-      <c r="C202" s="12"/>
+      <c r="C202" s="11"/>
       <c r="D202" s="11"/>
       <c r="E202" s="11"/>
       <c r="F202" s="11"/>
@@ -7464,7 +7464,7 @@
         <v>200</v>
       </c>
       <c r="B203" s="11"/>
-      <c r="C203" s="12"/>
+      <c r="C203" s="11"/>
       <c r="D203" s="11"/>
       <c r="E203" s="11"/>
       <c r="F203" s="11"/>
@@ -18625,7 +18625,7 @@
           <x14:formula1>
             <xm:f>'Lista desplegable'!$C$2:$C$34</xm:f>
           </x14:formula1>
-          <xm:sqref>J4:J203 C7:C203</xm:sqref>
+          <xm:sqref>J4:J203</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E7B19CF4-592D-4454-A5A1-52EDDACF947E}">
           <x14:formula1>

</xml_diff>